<commit_message>
md file és adatbázis
</commit_message>
<xml_diff>
--- a/Adatbázis.xlsx
+++ b/Adatbázis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tanulók\2024-25\13.D\Nagy Ferenc\Érettségi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F258179-F535-4ED7-9CDD-11E1EE0BB986}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C167473B-D9D6-4689-AB5A-3DCAEFE1AB98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kolcsonzes_Magyar" sheetId="1" r:id="rId1"/>
+    <sheet name="Kolcsonzes_Angol" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>muvek</t>
   </si>
@@ -113,12 +114,84 @@
   <si>
     <t>tanár</t>
   </si>
+  <si>
+    <t>poets</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <t>classId</t>
+  </si>
+  <si>
+    <t>rentals</t>
+  </si>
+  <si>
+    <t>specimen</t>
+  </si>
+  <si>
+    <t>specimenId</t>
+  </si>
+  <si>
+    <t>studentId</t>
+  </si>
+  <si>
+    <t>startingDate</t>
+  </si>
+  <si>
+    <t>endingDate</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>bookId</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>acquisitionDate</t>
+  </si>
+  <si>
+    <t>teacherId</t>
+  </si>
+  <si>
+    <t>olvasónaplók</t>
+  </si>
+  <si>
+    <t>diakVelemeny</t>
+  </si>
+  <si>
+    <t>ertekeles</t>
+  </si>
+  <si>
+    <t>valami</t>
+  </si>
+  <si>
+    <t>studentOpinion</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +205,14 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -155,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -178,17 +259,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -210,16 +310,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>519391</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>27535</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>217312</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44904</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -237,8 +337,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11058525" y="2628900"/>
-          <a:ext cx="1581150" cy="409575"/>
+          <a:off x="12464862" y="2201476"/>
+          <a:ext cx="1793421" cy="387163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -377,16 +477,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>313925</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>166326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>670273</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>18008</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -404,8 +504,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14306550" y="2686050"/>
-          <a:ext cx="1581150" cy="409575"/>
+          <a:off x="14354896" y="2710061"/>
+          <a:ext cx="1723465" cy="389565"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -544,16 +644,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123664</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>124384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>637214</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152960</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -571,8 +671,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12220575" y="3581400"/>
-          <a:ext cx="1581150" cy="409575"/>
+          <a:off x="12069135" y="3564590"/>
+          <a:ext cx="1802226" cy="387164"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -711,16 +811,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>23854</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>67474</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>441351</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -738,8 +838,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15849600" y="3876675"/>
-          <a:ext cx="1581150" cy="409575"/>
+          <a:off x="16799060" y="2062121"/>
+          <a:ext cx="1784615" cy="403172"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -878,16 +978,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>670273</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>67474</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>232603</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -913,9 +1013,77 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15887700" y="2890838"/>
-          <a:ext cx="752475" cy="985837"/>
+        <a:xfrm flipV="1">
+          <a:off x="16078361" y="2062121"/>
+          <a:ext cx="1613007" cy="842723"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 22340"/>
+            <a:gd name="adj2" fmla="val 127126"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1024777</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>313925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>124384</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Görbe összekötő 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81549BFB-CEC0-41FB-8959-660180AC32E5}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{87FCE781-16CE-4CC1-A4A9-C8F9885C69E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="5" idx="0"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{DC0FEBC1-FD83-4963-9BEF-AC7D93FAA5AE}" end="{FC1100EA-187F-4AF2-AC1E-02C7FBD99516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="12970248" y="2904844"/>
+          <a:ext cx="1384648" cy="659746"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector2">
           <a:avLst/>
@@ -943,47 +1111,50 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123664</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>127426</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>138673</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Görbe összekötő 8">
+        <xdr:cNvPr id="10" name="Görbe összekötő 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81549BFB-CEC0-41FB-8959-660180AC32E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE8F39F-9F2A-4A89-8F3E-8F127C87943C}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{87FCE781-16CE-4CC1-A4A9-C8F9885C69E9}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{81549BFB-CEC0-41FB-8959-660180AC32E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
-          <a:stCxn id="4" idx="1"/>
-          <a:endCxn id="5" idx="0"/>
+          <a:stCxn id="5" idx="1"/>
+          <a:endCxn id="3" idx="2"/>
           <a:extLst>
             <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
-              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{DC0FEBC1-FD83-4963-9BEF-AC7D93FAA5AE}" end="{FC1100EA-187F-4AF2-AC1E-02C7FBD99516}"/>
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{FC1100EA-187F-4AF2-AC1E-02C7FBD99516}" end="{D1E71B48-2862-4859-84F9-4E483B9E5426}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="13011150" y="2890838"/>
-          <a:ext cx="1295400" cy="690562"/>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="12069135" y="2588640"/>
+          <a:ext cx="1292438" cy="1169533"/>
         </a:xfrm>
-        <a:prstGeom prst="curvedConnector2">
-          <a:avLst/>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -17688"/>
+            <a:gd name="adj2" fmla="val 58276"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:headEnd type="triangle"/>
@@ -1008,81 +1179,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>200904</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>110459</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>428626</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>166689</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Görbe összekötő 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE8F39F-9F2A-4A89-8F3E-8F127C87943C}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{81549BFB-CEC0-41FB-8959-660180AC32E5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-          <a:stCxn id="5" idx="1"/>
-          <a:endCxn id="3" idx="2"/>
-          <a:extLst>
-            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
-              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{FC1100EA-187F-4AF2-AC1E-02C7FBD99516}" end="{D1E71B48-2862-4859-84F9-4E483B9E5426}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="11849101" y="3038476"/>
-          <a:ext cx="371475" cy="747713"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>557253</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>150238</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1100,8 +1206,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13868400" y="876300"/>
-          <a:ext cx="1581150" cy="409575"/>
+          <a:off x="14241875" y="1029341"/>
+          <a:ext cx="1723466" cy="398368"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1240,16 +1346,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>127427</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>130349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>200905</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>27535</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1276,8 +1382,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="12132469" y="892969"/>
-          <a:ext cx="1547812" cy="1924050"/>
+          <a:off x="13315249" y="1274850"/>
+          <a:ext cx="972951" cy="880302"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector2">
           <a:avLst/>
@@ -1305,16 +1411,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>557253</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>130349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>80963</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>441351</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>89766</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1341,12 +1447,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="15449550" y="1081088"/>
-          <a:ext cx="2076450" cy="3000375"/>
+          <a:off x="15965341" y="1228525"/>
+          <a:ext cx="2618334" cy="1035182"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -11009"/>
+            <a:gd name="adj1" fmla="val -8731"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1372,16 +1478,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561255</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>81004</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>234044</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>98373</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1399,8 +1505,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12668250" y="4838700"/>
-          <a:ext cx="1581150" cy="409575"/>
+          <a:off x="14602226" y="3700504"/>
+          <a:ext cx="1723465" cy="387163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1539,16 +1645,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>234044</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>232603</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95292</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1575,8 +1681,1477 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="14249400" y="4286250"/>
-          <a:ext cx="2486025" cy="757238"/>
+          <a:off x="16325691" y="2465293"/>
+          <a:ext cx="1365677" cy="1428793"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>127427</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561256</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95293</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Görbe összekötő 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA8831B-F998-471A-8E7F-3DB305432E42}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{27F6515F-3643-4557-8E77-4FF53CD72266}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="14" idx="1"/>
+          <a:endCxn id="3" idx="2"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{AEF5F3E6-020D-4824-B2BC-2E3AFA66EAC0}" end="{D1E71B48-2862-4859-84F9-4E483B9E5426}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="13361574" y="2588640"/>
+          <a:ext cx="1240653" cy="1305447"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Egyenes összekötő nyíllal 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A55EDBB4-84C0-4234-AA5E-09853A46250E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="962025" y="1295400"/>
+          <a:ext cx="2076450" cy="2343150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Egyenes összekötő nyíllal 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C4F03F6-1985-4B76-A7EA-1B32ADC37C5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="971550" y="2952750"/>
+          <a:ext cx="2476500" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Egyenes összekötő nyíllal 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69F8B870-952F-4E0C-AC84-4E8C547497BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1295400" y="1285875"/>
+          <a:ext cx="5724525" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Egyenes összekötő nyíllal 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB50DC16-799F-447D-BFEB-241FE4C06E33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6181725" y="1666875"/>
+          <a:ext cx="1581150" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>616323</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="Egyenes összekötő nyíllal 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C5E4F2-F006-483D-95AD-B54F9E560AD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1299882" y="1288676"/>
+          <a:ext cx="6051177" cy="2891118"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>63954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>6083</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>81323</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Téglalap 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63602419-4CD9-4ED8-8586-30BFB352B70D}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{AA3620C4-BA49-BB15-B8BA-8AE81A40ECAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11721353" y="2237895"/>
+          <a:ext cx="1787818" cy="387163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>books</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>472488</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>103575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>150879</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>134552</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Téglalap 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F73560FE-703A-4692-B66B-DD343A1F3721}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D1E71B48-2862-4859-84F9-4E483B9E5426}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14435017" y="2468016"/>
+          <a:ext cx="1729068" cy="389565"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>rental</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57551</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>159683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>564377</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>188259</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Téglalap 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6501859-848F-4065-9313-1E8F7ADDD75B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DC0FEBC1-FD83-4963-9BEF-AC7D93FAA5AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11924580" y="3599889"/>
+          <a:ext cx="1795503" cy="387164"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>specimen</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95009</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68034</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>510827</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101413</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Téglalap 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB35556A-C15D-4042-AE32-7534C87A5861}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FC1100EA-187F-4AF2-AC1E-02C7FBD99516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16791774" y="2241975"/>
+          <a:ext cx="1782935" cy="403173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>users</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>150879</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68034</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>302918</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119064</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Görbe összekötő 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B87ADEA7-E22A-4AE2-8287-939B18513A99}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{AAFDA631-19DB-49BB-9DA2-53980D0990AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="5" idx="0"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{DC0FEBC1-FD83-4963-9BEF-AC7D93FAA5AE}" end="{AAFDA631-19DB-49BB-9DA2-53980D0990AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16164085" y="2241975"/>
+          <a:ext cx="1519157" cy="420824"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 20659"/>
+            <a:gd name="adj2" fmla="val 154322"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>955304</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>472489</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>159683</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Görbe összekötő 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B0F4D8-D07E-4E45-AD95-F1214FF0149C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{87FCE781-16CE-4CC1-A4A9-C8F9885C69E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="3" idx="1"/>
+          <a:endCxn id="4" idx="0"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{DC0FEBC1-FD83-4963-9BEF-AC7D93FAA5AE}" end="{FC1100EA-187F-4AF2-AC1E-02C7FBD99516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="12822333" y="2662799"/>
+          <a:ext cx="1612685" cy="937090"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>81324</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1207673</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>173972</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Görbe összekötő 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D54623F-E729-4BB7-8D33-7E8A13C4B39B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{81549BFB-CEC0-41FB-8959-660180AC32E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="2" idx="2"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{FC1100EA-187F-4AF2-AC1E-02C7FBD99516}" end="{D1E71B48-2862-4859-84F9-4E483B9E5426}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="11924579" y="2625059"/>
+          <a:ext cx="1150123" cy="1168413"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -19876"/>
+            <a:gd name="adj2" fmla="val 58284"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>89966</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>79642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>440711</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>119422</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Téglalap 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2A53CE1-9A81-4A3D-B200-EE02A26FC614}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{6DE8F39F-9F2A-4A89-8F3E-8F127C87943C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13605941" y="1003567"/>
+          <a:ext cx="1722345" cy="401730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>classes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1207674</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>99533</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>89966</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>63954</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Görbe összekötő 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67AB7EFD-1FCB-44B7-B57C-66235ECA84E5}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A76DF5FF-1CE2-4D35-ADA2-9100F4C9D462}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="2" idx="0"/>
+          <a:endCxn id="9" idx="1"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{D1E71B48-2862-4859-84F9-4E483B9E5426}" end="{A76DF5FF-1CE2-4D35-ADA2-9100F4C9D462}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="12584065" y="1228906"/>
+          <a:ext cx="1040186" cy="977792"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector2">
           <a:avLst/>
@@ -1605,49 +3180,637 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>440711</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>99533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>90489</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>510827</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>79121</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Görbe összekötő 15">
+        <xdr:cNvPr id="11" name="Görbe összekötő 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA8831B-F998-471A-8E7F-3DB305432E42}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58768AD5-68EA-4B8B-B669-0749A946E0B6}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{27F6515F-3643-4557-8E77-4FF53CD72266}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4CB01B13-36F5-4DCE-86CC-739038B819AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
-          <a:stCxn id="14" idx="1"/>
-          <a:endCxn id="3" idx="2"/>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="9" idx="3"/>
           <a:extLst>
             <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
-              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{AEF5F3E6-020D-4824-B2BC-2E3AFA66EAC0}" end="{D1E71B48-2862-4859-84F9-4E483B9E5426}"/>
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{AAFDA631-19DB-49BB-9DA2-53980D0990AA}" end="{A76DF5FF-1CE2-4D35-ADA2-9100F4C9D462}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="11944350" y="3038476"/>
-          <a:ext cx="723900" cy="2005013"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="15770358" y="1197709"/>
+          <a:ext cx="2804351" cy="1245853"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -8152"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>302959</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>112381</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>658745</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142636</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Téglalap 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F015BF4-4BA1-49D4-AADC-278E0FE87EFB}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{57BF2EFD-1032-43D4-A49F-2F4E7128B3FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14265488" y="3731881"/>
+          <a:ext cx="1722904" cy="400049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>r</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>eading diar</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>ies</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>658745</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>302918</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133112</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Görbe összekötő 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65181972-9BA1-445B-8723-BE6543F2E22C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{AEF5F3E6-020D-4824-B2BC-2E3AFA66EAC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="12" idx="3"/>
+          <a:endCxn id="5" idx="2"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{AEF5F3E6-020D-4824-B2BC-2E3AFA66EAC0}" end="{AAFDA631-19DB-49BB-9DA2-53980D0990AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15988392" y="2645148"/>
+          <a:ext cx="1694850" cy="1286758"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector2">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1207675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>81323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>302960</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133112</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Görbe összekötő 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FBFCD1B-F748-474F-843E-E5CF392158EF}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{27F6515F-3643-4557-8E77-4FF53CD72266}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="12" idx="1"/>
+          <a:endCxn id="2" idx="2"/>
+          <a:extLst>
+            <a:ext uri="{5F17804C-33F3-41E3-A699-7DCFA2EF7971}">
+              <a16:cxnDERefs xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" st="{AEF5F3E6-020D-4824-B2BC-2E3AFA66EAC0}" end="{D1E71B48-2862-4859-84F9-4E483B9E5426}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="13074704" y="2625058"/>
+          <a:ext cx="1190785" cy="1306848"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Egyenes összekötő nyíllal 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{341CA767-28C2-45EA-A804-9E9782C04FB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="962025" y="1304925"/>
+          <a:ext cx="2505075" cy="2343150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Egyenes összekötő nyíllal 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0036F578-1149-4B9C-9309-C084C5E5084A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="971550" y="2962275"/>
+          <a:ext cx="2905125" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>425823</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>139513</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3362</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Egyenes összekötő nyíllal 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2F21D28-779D-4844-8ACB-D1AAE79E3967}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019735" y="1299882"/>
+          <a:ext cx="7154396" cy="698127"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Egyenes összekötő nyíllal 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{508FFDF3-B355-4496-8F78-E0B71A588A7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7000875" y="1666875"/>
+          <a:ext cx="1581150" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>672353</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>168088</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Egyenes összekötő nyíllal 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65BEFE78-1072-45AC-B7FB-82272F12263D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266265" y="1288676"/>
+          <a:ext cx="5995147" cy="2868706"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1987,43 +4150,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:Q17"/>
+  <dimension ref="B3:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="28.75" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
     <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.25" customWidth="1"/>
     <col min="12" max="12" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.875" customWidth="1"/>
     <col min="14" max="14" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17">
+    <row r="3" spans="2:13">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="N3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="2:17" ht="15">
+    <row r="4" spans="2:13" ht="15">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2036,30 +4191,15 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="2:17">
+    <row r="5" spans="2:13" ht="15">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2072,25 +4212,23 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1">
+      <c r="I5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="2:17">
+    <row r="6" spans="2:13">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -2103,25 +4241,23 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="1">
-        <v>2</v>
-      </c>
       <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="N6" s="1">
+      <c r="J6" s="1">
         <v>2</v>
       </c>
-      <c r="O6" s="1">
-        <v>2</v>
-      </c>
-      <c r="P6" s="1">
-        <v>4</v>
+      <c r="K6" s="1">
+        <v>45</v>
+      </c>
+      <c r="L6" s="9">
+        <v>45599</v>
+      </c>
+      <c r="M6" s="9">
+        <v>45630</v>
       </c>
     </row>
-    <row r="7" spans="2:17">
+    <row r="7" spans="2:13">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -2132,35 +4268,57 @@
       <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="H7" s="1">
-        <v>3</v>
-      </c>
       <c r="I7" s="1">
         <v>2</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="N7" s="1">
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>23</v>
+      </c>
+      <c r="L7" s="9">
+        <v>45600</v>
+      </c>
+      <c r="M7" s="9">
+        <v>45631</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="I8" s="1">
         <v>3</v>
       </c>
-      <c r="O7" s="1">
+      <c r="J8" s="1">
         <v>3</v>
       </c>
-      <c r="P7" s="1">
-        <v>5</v>
+      <c r="K8" s="1">
+        <v>23</v>
+      </c>
+      <c r="L8" s="9">
+        <v>45601</v>
+      </c>
+      <c r="M8" s="9">
+        <v>45632</v>
       </c>
     </row>
-    <row r="8" spans="2:17">
-      <c r="H8" s="1">
+    <row r="9" spans="2:13">
+      <c r="I9" s="1">
         <v>4</v>
       </c>
-      <c r="I8" s="1">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="J9" s="1">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>65</v>
+      </c>
+      <c r="L9" s="9">
+        <v>45602</v>
+      </c>
+      <c r="M9" s="9">
+        <v>45633</v>
+      </c>
     </row>
-    <row r="12" spans="2:17">
+    <row r="12" spans="2:13">
       <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
@@ -2168,14 +4326,13 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="2:17" ht="15">
+    <row r="13" spans="2:13" ht="15">
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2192,19 +4349,16 @@
         <v>3</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:17">
+    <row r="14" spans="2:13">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -2219,15 +4373,16 @@
         <v>1</v>
       </c>
       <c r="I14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1">
-        <v>45</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+        <v>4900</v>
+      </c>
+      <c r="K14" s="9">
+        <v>44077</v>
+      </c>
     </row>
-    <row r="15" spans="2:17">
+    <row r="15" spans="2:13">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -2241,12 +4396,17 @@
       <c r="H15" s="1">
         <v>2</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4900</v>
+      </c>
+      <c r="K15" s="9">
+        <v>44077</v>
+      </c>
     </row>
-    <row r="16" spans="2:17">
+    <row r="16" spans="2:13">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -2260,19 +4420,553 @@
       <c r="H16" s="1">
         <v>3</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="I16" s="1">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1">
+        <v>4900</v>
+      </c>
+      <c r="K16" s="9">
+        <v>44077</v>
+      </c>
     </row>
-    <row r="17" spans="8:12">
+    <row r="17" spans="2:11">
       <c r="H17" s="1">
         <v>4</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4900</v>
+      </c>
+      <c r="K17" s="9">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:11" ht="15">
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="2:11" ht="15">
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="F26" s="6">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="F27" s="6">
+        <v>2</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="F28" s="6">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="6">
+        <v>2</v>
+      </c>
+      <c r="I28" s="6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37A8F50-268A-44E3-9D76-18244422357E}">
+  <dimension ref="B3:M28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="28.75" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
+    <col min="11" max="11" width="17.25" customWidth="1"/>
+    <col min="12" max="12" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.875" customWidth="1"/>
+    <col min="14" max="14" width="10.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13">
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="2:13" ht="15">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="2:13" ht="15">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>45</v>
+      </c>
+      <c r="L6" s="9">
+        <v>45599</v>
+      </c>
+      <c r="M6" s="9">
+        <v>45630</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>23</v>
+      </c>
+      <c r="L7" s="9">
+        <v>45600</v>
+      </c>
+      <c r="M7" s="9">
+        <v>45631</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1">
+        <v>23</v>
+      </c>
+      <c r="L8" s="9">
+        <v>45601</v>
+      </c>
+      <c r="M8" s="9">
+        <v>45632</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="I9" s="1">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>65</v>
+      </c>
+      <c r="L9" s="9">
+        <v>45602</v>
+      </c>
+      <c r="M9" s="9">
+        <v>45633</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:13" ht="15">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4900</v>
+      </c>
+      <c r="K14" s="9">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4900</v>
+      </c>
+      <c r="K15" s="9">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1">
+        <v>4900</v>
+      </c>
+      <c r="K16" s="9">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="H17" s="1">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4900</v>
+      </c>
+      <c r="K17" s="9">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:11" ht="15">
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="2:11" ht="15">
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="F26" s="6">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="F27" s="6">
+        <v>2</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="F28" s="6">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6">
+        <v>2</v>
+      </c>
+      <c r="I28" s="6">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2281,6 +4975,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c7c92ca0-021c-40ca-94a6-a2e5f6245384">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x01010064BA54B0C393A2489552B8F9332406A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="44c5ac6e7392cc0f6ba3a968409ffb51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c7c92ca0-021c-40ca-94a6-a2e5f6245384" xmlns:ns3="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b89e65a35ff79a095a034a3ad1d32fa9" ns2:_="" ns3:_="">
     <xsd:import namespace="c7c92ca0-021c-40ca-94a6-a2e5f6245384"/>
@@ -2481,27 +5195,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c7c92ca0-021c-40ca-94a6-a2e5f6245384">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4703BB6-11CC-4E01-BAEE-485DB49CD518}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9A34FBF-C707-4416-8F50-87DEE65F10DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c7c92ca0-021c-40ca-94a6-a2e5f6245384"/>
+    <ds:schemaRef ds:uri="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E4E68B4-4024-41CF-AD75-32875475BC7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2518,23 +5231,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9A34FBF-C707-4416-8F50-87DEE65F10DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c7c92ca0-021c-40ca-94a6-a2e5f6245384"/>
-    <ds:schemaRef ds:uri="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4703BB6-11CC-4E01-BAEE-485DB49CD518}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Összefoglaló javítása, groups, roles, users táblázat
</commit_message>
<xml_diff>
--- a/Adatbázis.xlsx
+++ b/Adatbázis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tanulók\2024-25\13.D\Nagy Ferenc\Érettségi\Kölcsönzés\Kolcsonzes_Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E965CB3C-D24E-406E-AB1F-F9DD212EB1D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6133DE7C-0CE9-45E0-8C13-56E1654CDFD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kolcsonzes_Magyar" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>muvek</t>
   </si>
@@ -115,9 +115,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>books</t>
-  </si>
-  <si>
     <t>classId</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>classes</t>
   </si>
   <si>
     <t>bookId</t>
@@ -194,6 +188,15 @@
   </si>
   <si>
     <t>roles</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>groupId</t>
   </si>
 </sst>
 </file>
@@ -3182,15 +3185,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>89966</xdr:colOff>
+      <xdr:colOff>33937</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>79642</xdr:rowOff>
+      <xdr:rowOff>90848</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>440711</xdr:colOff>
+      <xdr:colOff>384682</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>119422</xdr:rowOff>
+      <xdr:rowOff>130628</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3208,8 +3211,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13605941" y="1003567"/>
-          <a:ext cx="1722345" cy="401730"/>
+          <a:off x="14130937" y="1009730"/>
+          <a:ext cx="1717863" cy="398369"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3339,7 +3342,7 @@
               </a:solidFill>
               <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>classes</a:t>
+            <a:t>groups</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -3355,15 +3358,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1207674</xdr:colOff>
+      <xdr:colOff>1207673</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>99533</xdr:rowOff>
+      <xdr:rowOff>110740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>89966</xdr:colOff>
+      <xdr:colOff>33936</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>63954</xdr:rowOff>
+      <xdr:rowOff>63955</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3390,8 +3393,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="12584065" y="1228906"/>
-          <a:ext cx="1040186" cy="977792"/>
+          <a:off x="13155565" y="1262524"/>
+          <a:ext cx="1028980" cy="921763"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector2">
           <a:avLst/>
@@ -3420,9 +3423,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>440711</xdr:colOff>
+      <xdr:colOff>384682</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>99533</xdr:rowOff>
+      <xdr:rowOff>110739</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
@@ -3455,12 +3458,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="15770358" y="1197709"/>
-          <a:ext cx="2804351" cy="1245853"/>
+          <a:off x="15848800" y="1208915"/>
+          <a:ext cx="2860380" cy="1234647"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -8152"/>
+            <a:gd name="adj1" fmla="val -7992"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -4625,7 +4628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -4814,7 +4817,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>6</v>
@@ -4960,7 +4963,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -4980,13 +4983,13 @@
         <v>3</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:11">
@@ -4994,7 +4997,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H26" s="6">
         <v>1</v>
@@ -5005,14 +5008,14 @@
     </row>
     <row r="27" spans="2:11">
       <c r="B27" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="7"/>
       <c r="F27" s="6">
         <v>2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H27" s="6">
         <v>1</v>
@@ -5026,13 +5029,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F28" s="6">
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H28" s="6">
         <v>2</v>
@@ -5062,7 +5065,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -5076,8 +5079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37A8F50-268A-44E3-9D76-18244422357E}">
   <dimension ref="B3:M33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5097,7 +5100,7 @@
   <sheetData>
     <row r="3" spans="2:13">
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5114,10 +5117,10 @@
         <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -5141,16 +5144,16 @@
         <v>3</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -5251,7 +5254,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -5262,25 +5265,25 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -5371,7 +5374,7 @@
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -5382,10 +5385,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="4"/>
     </row>
@@ -5411,7 +5414,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -5431,13 +5434,13 @@
         <v>3</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:11">
@@ -5478,7 +5481,7 @@
     </row>
     <row r="29" spans="2:11">
       <c r="B29" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="7"/>
     </row>
@@ -5487,7 +5490,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="2:11">
@@ -5511,7 +5514,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -5530,6 +5533,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c7c92ca0-021c-40ca-94a6-a2e5f6245384">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x01010064BA54B0C393A2489552B8F9332406A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="44c5ac6e7392cc0f6ba3a968409ffb51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c7c92ca0-021c-40ca-94a6-a2e5f6245384" xmlns:ns3="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b89e65a35ff79a095a034a3ad1d32fa9" ns2:_="" ns3:_="">
     <xsd:import namespace="c7c92ca0-021c-40ca-94a6-a2e5f6245384"/>
@@ -5730,17 +5744,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c7c92ca0-021c-40ca-94a6-a2e5f6245384">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4703BB6-11CC-4E01-BAEE-485DB49CD518}">
   <ds:schemaRefs>
@@ -5750,6 +5753,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9A34FBF-C707-4416-8F50-87DEE65F10DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c7c92ca0-021c-40ca-94a6-a2e5f6245384"/>
+    <ds:schemaRef ds:uri="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E4E68B4-4024-41CF-AD75-32875475BC7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5766,15 +5780,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9A34FBF-C707-4416-8F50-87DEE65F10DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c7c92ca0-021c-40ca-94a6-a2e5f6245384"/>
-    <ds:schemaRef ds:uri="517a9ed4-7eb6-4d79-bb13-f742afa9ee4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>